<commit_message>
Included the cell formatting feature
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a3b1b6b23fc8a11/ドキュメント/UiPath/ARPA-Excel-Activities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_6F12DD367C351707A7D5F15062166DD5C216F2C6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BCC6B1A-AA14-4E51-BFEB-89F4777A6349}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_6F12DD369B1D5D1C4334EBEBBA419F49C5EEF3F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A45B0F7-1826-4667-B885-52D0D07DD00A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,9 @@
     <t>BookID</t>
   </si>
   <si>
+    <t>Borrower's Name</t>
+  </si>
+  <si>
     <t>Book Name</t>
   </si>
   <si>
@@ -37,18 +40,15 @@
     <t>Fine Charges</t>
   </si>
   <si>
-    <t>Borrower's Name_1</t>
-  </si>
-  <si>
     <t>Profession</t>
   </si>
   <si>
+    <t>Mike</t>
+  </si>
+  <si>
     <t>The Paying Guests</t>
   </si>
   <si>
-    <t>Mike</t>
-  </si>
-  <si>
     <t>STUDENT</t>
   </si>
   <si>
@@ -70,12 +70,12 @@
     <t>A Town Like Alice</t>
   </si>
   <si>
+    <t>Doug</t>
+  </si>
+  <si>
     <t>Alice's Adventures in Wonderland by Lewis Carroll</t>
   </si>
   <si>
-    <t>Doug</t>
-  </si>
-  <si>
     <t>All Quiet on the Western Front</t>
   </si>
   <si>
@@ -91,18 +91,18 @@
     <t>The Handmaid's Tale</t>
   </si>
   <si>
+    <t>Rick</t>
+  </si>
+  <si>
     <t>Animal Farm</t>
   </si>
   <si>
-    <t>Rick</t>
+    <t>Cooper</t>
   </si>
   <si>
     <t>Atonement</t>
   </si>
   <si>
-    <t>Cooper</t>
-  </si>
-  <si>
     <t>Barney's Version</t>
   </si>
   <si>
@@ -121,12 +121,12 @@
     <t>The Giver</t>
   </si>
   <si>
+    <t>Penny</t>
+  </si>
+  <si>
     <t>Brave New World</t>
   </si>
   <si>
-    <t>Penny</t>
-  </si>
-  <si>
     <t>Anna Karenina</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>The Chrysalids</t>
   </si>
   <si>
+    <t>Michael</t>
+  </si>
+  <si>
     <t>Grapes of Wrath</t>
   </si>
   <si>
-    <t>Michael</t>
-  </si>
-  <si>
     <t>Great Expectations</t>
   </si>
   <si>
@@ -172,12 +172,12 @@
     <t>Harry Potter and the Sorcerer's Stone</t>
   </si>
   <si>
+    <t>Max</t>
+  </si>
+  <si>
     <t>The Help</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>The Hitchiker's Guide to the Galaxy</t>
   </si>
   <si>
@@ -211,12 +211,12 @@
     <t>The Lion, the Witch, and the Wardrobe</t>
   </si>
   <si>
+    <t>Dick</t>
+  </si>
+  <si>
     <t>The Little Prince</t>
   </si>
   <si>
-    <t>Dick</t>
-  </si>
-  <si>
     <t>Lolita</t>
   </si>
   <si>
@@ -229,12 +229,12 @@
     <t>Maus</t>
   </si>
   <si>
+    <t>Robin</t>
+  </si>
+  <si>
     <t>North and South</t>
   </si>
   <si>
-    <t>Robin</t>
-  </si>
-  <si>
     <t>Of Mice and Men</t>
   </si>
   <si>
@@ -244,12 +244,12 @@
     <t>One Day in the Life of Ivan Denisovich</t>
   </si>
   <si>
+    <t>Jackson</t>
+  </si>
+  <si>
     <t>Romance of the Three Kingdoms</t>
   </si>
   <si>
-    <t>Jackson</t>
-  </si>
-  <si>
     <t>The Shining</t>
   </si>
   <si>
@@ -259,34 +259,34 @@
     <t>The Sound and the Fury</t>
   </si>
   <si>
+    <t>Leonard</t>
+  </si>
+  <si>
     <t>The Sun Also Rises</t>
   </si>
   <si>
-    <t>Leonard</t>
-  </si>
-  <si>
     <t>Tess of the D'Urbervilles</t>
   </si>
   <si>
     <t>Things Fall Apart</t>
   </si>
   <si>
+    <t>Alex</t>
+  </si>
+  <si>
     <t>To Kill A Mockingbird</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>The Trial</t>
   </si>
   <si>
     <t>Tropic of Cancer</t>
   </si>
   <si>
+    <t>Albert</t>
+  </si>
+  <si>
     <t>The Unbearable Lightness of Being</t>
-  </si>
-  <si>
-    <t>Albert</t>
   </si>
   <si>
     <t>War and Peace</t>
@@ -307,12 +307,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -327,9 +339,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,9 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -670,17 +682,17 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
-        <v>44063</v>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E2" s="1">
         <v>44064</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2">
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -691,19 +703,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>44044</v>
       </c>
-      <c r="D3" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F3">
         <v>190</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -714,19 +726,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44051</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>44062</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>110</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -737,19 +749,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>44047</v>
       </c>
-      <c r="D5" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E5">
+      <c r="E5" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F5">
         <v>160</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -760,19 +772,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>44053</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>44060</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -783,19 +795,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>44043</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>44052</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -806,19 +818,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1">
-        <v>44063</v>
-      </c>
       <c r="D8" s="1">
         <v>44063</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
+      <c r="E8" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -831,17 +843,17 @@
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1">
         <v>44043</v>
       </c>
-      <c r="D9" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E9">
+      <c r="E9" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F9">
         <v>200</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -852,19 +864,19 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>44017</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>44062</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>450</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -875,19 +887,19 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>44047</v>
       </c>
-      <c r="D11" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E11">
+      <c r="E11" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F11">
         <v>160</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -898,19 +910,19 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>44044</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>44060</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>160</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
       </c>
       <c r="G12" t="s">
         <v>9</v>
@@ -921,19 +933,19 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>44044</v>
       </c>
-      <c r="D13" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E13">
+      <c r="E13" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F13">
         <v>190</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -944,19 +956,19 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1">
-        <v>44063</v>
-      </c>
       <c r="D14" s="1">
         <v>44063</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
+      <c r="E14" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
@@ -969,17 +981,17 @@
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
         <v>44047</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>44052</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
+      <c r="F15">
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
@@ -992,17 +1004,17 @@
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
         <v>44053</v>
       </c>
-      <c r="D16" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E16">
+      <c r="E16" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F16">
         <v>100</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
@@ -1013,19 +1025,19 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>44043</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>44048</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
+      <c r="F17">
+        <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>9</v>
@@ -1036,19 +1048,19 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>44017</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>44059</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>420</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
       </c>
       <c r="G18" t="s">
         <v>9</v>
@@ -1059,19 +1071,19 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="1">
-        <v>44063</v>
-      </c>
       <c r="D19" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E19" s="1">
         <v>44070</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
+      <c r="F19">
+        <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>9</v>
@@ -1082,19 +1094,19 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>44044</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>44064</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>200</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
@@ -1105,19 +1117,19 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>44044</v>
       </c>
-      <c r="D21" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E21">
+      <c r="E21" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F21">
         <v>190</v>
-      </c>
-      <c r="F21" t="s">
-        <v>26</v>
       </c>
       <c r="G21" t="s">
         <v>9</v>
@@ -1128,19 +1140,19 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="1">
-        <v>44063</v>
-      </c>
       <c r="D22" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E22" s="1">
         <v>44062</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
+      <c r="F22">
+        <v>0</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
@@ -1153,17 +1165,17 @@
       <c r="B23" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1">
         <v>44047</v>
       </c>
-      <c r="D23" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E23">
+      <c r="E23" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F23">
         <v>160</v>
-      </c>
-      <c r="F23" t="s">
-        <v>34</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
@@ -1174,19 +1186,19 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>44053</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>44060</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
+      <c r="F24">
+        <v>0</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -1197,19 +1209,19 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>44043</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>44052</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>90</v>
-      </c>
-      <c r="F25" t="s">
-        <v>34</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
@@ -1220,19 +1232,19 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="1">
-        <v>44063</v>
-      </c>
       <c r="D26" s="1">
         <v>44063</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
+      <c r="E26" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -1243,19 +1255,19 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>44047</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>44064</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>170</v>
-      </c>
-      <c r="F27" t="s">
-        <v>34</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
@@ -1266,19 +1278,19 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="1">
-        <v>44063</v>
-      </c>
       <c r="D28" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E28" s="1">
         <v>44064</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>34</v>
+      <c r="F28">
+        <v>0</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -1289,19 +1301,19 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>44044</v>
       </c>
-      <c r="D29" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E29">
+      <c r="E29" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F29">
         <v>190</v>
-      </c>
-      <c r="F29" t="s">
-        <v>34</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
@@ -1312,19 +1324,19 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>44051</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>44062</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>110</v>
-      </c>
-      <c r="F30" t="s">
-        <v>34</v>
       </c>
       <c r="G30" t="s">
         <v>9</v>
@@ -1337,17 +1349,17 @@
       <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="1">
         <v>44017</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>44062</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>450</v>
-      </c>
-      <c r="F31" t="s">
-        <v>43</v>
       </c>
       <c r="G31" t="s">
         <v>9</v>
@@ -1358,19 +1370,19 @@
         <v>48</v>
       </c>
       <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>44047</v>
       </c>
-      <c r="D32" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E32">
+      <c r="E32" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F32">
         <v>160</v>
-      </c>
-      <c r="F32" t="s">
-        <v>43</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
@@ -1381,19 +1393,19 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>44044</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>44060</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>160</v>
-      </c>
-      <c r="F33" t="s">
-        <v>43</v>
       </c>
       <c r="G33" t="s">
         <v>9</v>
@@ -1404,19 +1416,19 @@
         <v>50</v>
       </c>
       <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>44044</v>
       </c>
-      <c r="D34" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E34">
+      <c r="E34" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F34">
         <v>190</v>
-      </c>
-      <c r="F34" t="s">
-        <v>43</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
@@ -1427,19 +1439,19 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="1">
-        <v>44063</v>
-      </c>
       <c r="D35" s="1">
         <v>44063</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>43</v>
+      <c r="E35" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
       </c>
       <c r="G35" t="s">
         <v>9</v>
@@ -1450,19 +1462,19 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>44047</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>44052</v>
       </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>43</v>
+      <c r="F36">
+        <v>0</v>
       </c>
       <c r="G36" t="s">
         <v>9</v>
@@ -1473,19 +1485,19 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>44053</v>
       </c>
-      <c r="D37" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E37">
+      <c r="E37" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F37">
         <v>100</v>
-      </c>
-      <c r="F37" t="s">
-        <v>43</v>
       </c>
       <c r="G37" t="s">
         <v>9</v>
@@ -1498,17 +1510,17 @@
       <c r="B38" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="1">
         <v>44043</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>44048</v>
       </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
-        <v>51</v>
+      <c r="F38">
+        <v>0</v>
       </c>
       <c r="G38" t="s">
         <v>9</v>
@@ -1519,19 +1531,19 @@
         <v>55</v>
       </c>
       <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>44017</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>44059</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>420</v>
-      </c>
-      <c r="F39" t="s">
-        <v>51</v>
       </c>
       <c r="G39" t="s">
         <v>9</v>
@@ -1542,19 +1554,19 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="1">
-        <v>44063</v>
-      </c>
       <c r="D40" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E40" s="1">
         <v>44070</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>51</v>
+      <c r="F40">
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
@@ -1565,19 +1577,19 @@
         <v>57</v>
       </c>
       <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>44044</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>44064</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>200</v>
-      </c>
-      <c r="F41" t="s">
-        <v>51</v>
       </c>
       <c r="G41" t="s">
         <v>9</v>
@@ -1588,19 +1600,19 @@
         <v>58</v>
       </c>
       <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>44044</v>
       </c>
-      <c r="D42" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E42">
+      <c r="E42" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F42">
         <v>190</v>
-      </c>
-      <c r="F42" t="s">
-        <v>51</v>
       </c>
       <c r="G42" t="s">
         <v>9</v>
@@ -1611,19 +1623,19 @@
         <v>59</v>
       </c>
       <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="1">
-        <v>44063</v>
-      </c>
       <c r="D43" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E43" s="1">
         <v>44062</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>51</v>
+      <c r="F43">
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>9</v>
@@ -1634,19 +1646,19 @@
         <v>60</v>
       </c>
       <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>44047</v>
       </c>
-      <c r="D44" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E44">
+      <c r="E44" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F44">
         <v>160</v>
-      </c>
-      <c r="F44" t="s">
-        <v>51</v>
       </c>
       <c r="G44" t="s">
         <v>9</v>
@@ -1657,19 +1669,19 @@
         <v>61</v>
       </c>
       <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>44053</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>44060</v>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
-        <v>51</v>
+      <c r="F45">
+        <v>0</v>
       </c>
       <c r="G45" t="s">
         <v>9</v>
@@ -1680,19 +1692,19 @@
         <v>62</v>
       </c>
       <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>44043</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>44052</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>90</v>
-      </c>
-      <c r="F46" t="s">
-        <v>51</v>
       </c>
       <c r="G46" t="s">
         <v>9</v>
@@ -1703,19 +1715,19 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="1">
-        <v>44063</v>
-      </c>
       <c r="D47" s="1">
         <v>44063</v>
       </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" t="s">
-        <v>51</v>
+      <c r="E47" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47" t="s">
         <v>9</v>
@@ -1726,19 +1738,19 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>44047</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>44064</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>170</v>
-      </c>
-      <c r="F48" t="s">
-        <v>51</v>
       </c>
       <c r="G48" t="s">
         <v>9</v>
@@ -1749,19 +1761,19 @@
         <v>65</v>
       </c>
       <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="1">
-        <v>44063</v>
-      </c>
       <c r="D49" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E49" s="1">
         <v>44064</v>
       </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49" t="s">
-        <v>51</v>
+      <c r="F49">
+        <v>0</v>
       </c>
       <c r="G49" t="s">
         <v>9</v>
@@ -1774,17 +1786,17 @@
       <c r="B50" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="1">
         <v>44044</v>
       </c>
-      <c r="D50" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E50">
+      <c r="E50" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F50">
         <v>190</v>
-      </c>
-      <c r="F50" t="s">
-        <v>64</v>
       </c>
       <c r="G50" t="s">
         <v>9</v>
@@ -1795,19 +1807,19 @@
         <v>67</v>
       </c>
       <c r="B51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>44051</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>44062</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>110</v>
-      </c>
-      <c r="F51" t="s">
-        <v>64</v>
       </c>
       <c r="G51" t="s">
         <v>9</v>
@@ -1818,19 +1830,19 @@
         <v>68</v>
       </c>
       <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>44047</v>
       </c>
-      <c r="D52" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E52">
+      <c r="E52" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F52">
         <v>160</v>
-      </c>
-      <c r="F52" t="s">
-        <v>64</v>
       </c>
       <c r="G52" t="s">
         <v>9</v>
@@ -1841,19 +1853,19 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>44053</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>44060</v>
       </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
-        <v>64</v>
+      <c r="F53">
+        <v>0</v>
       </c>
       <c r="G53" t="s">
         <v>9</v>
@@ -1864,19 +1876,19 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D54" s="1">
         <v>44043</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>44052</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>90</v>
-      </c>
-      <c r="F54" t="s">
-        <v>64</v>
       </c>
       <c r="G54" t="s">
         <v>9</v>
@@ -1889,17 +1901,17 @@
       <c r="B55" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="1">
         <v>44043</v>
       </c>
-      <c r="D55" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E55">
+      <c r="E55" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F55">
         <v>200</v>
-      </c>
-      <c r="F55" t="s">
-        <v>70</v>
       </c>
       <c r="G55" t="s">
         <v>9</v>
@@ -1910,19 +1922,19 @@
         <v>79</v>
       </c>
       <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>44017</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>44062</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>450</v>
-      </c>
-      <c r="F56" t="s">
-        <v>70</v>
       </c>
       <c r="G56" t="s">
         <v>9</v>
@@ -1933,19 +1945,19 @@
         <v>80</v>
       </c>
       <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D57" s="1">
         <v>44047</v>
       </c>
-      <c r="D57" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E57">
+      <c r="E57" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F57">
         <v>160</v>
-      </c>
-      <c r="F57" t="s">
-        <v>70</v>
       </c>
       <c r="G57" t="s">
         <v>9</v>
@@ -1956,19 +1968,19 @@
         <v>81</v>
       </c>
       <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>44044</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>44060</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>160</v>
-      </c>
-      <c r="F58" t="s">
-        <v>70</v>
       </c>
       <c r="G58" t="s">
         <v>9</v>
@@ -1981,17 +1993,17 @@
       <c r="B59" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="1">
         <v>44043</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>44048</v>
       </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
-        <v>75</v>
+      <c r="F59">
+        <v>0</v>
       </c>
       <c r="G59" t="s">
         <v>9</v>
@@ -2002,19 +2014,19 @@
         <v>87</v>
       </c>
       <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>44017</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>44059</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>420</v>
-      </c>
-      <c r="F60" t="s">
-        <v>75</v>
       </c>
       <c r="G60" t="s">
         <v>9</v>
@@ -2025,19 +2037,19 @@
         <v>88</v>
       </c>
       <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="1">
-        <v>44063</v>
-      </c>
       <c r="D61" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E61" s="1">
         <v>44070</v>
       </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
-        <v>75</v>
+      <c r="F61">
+        <v>0</v>
       </c>
       <c r="G61" t="s">
         <v>9</v>
@@ -2048,19 +2060,19 @@
         <v>89</v>
       </c>
       <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>44044</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>44064</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>200</v>
-      </c>
-      <c r="F62" t="s">
-        <v>75</v>
       </c>
       <c r="G62" t="s">
         <v>9</v>
@@ -2073,17 +2085,17 @@
       <c r="B63" t="s">
         <v>79</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="1">
         <v>44044</v>
       </c>
-      <c r="D63" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E63">
+      <c r="E63" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F63">
         <v>190</v>
-      </c>
-      <c r="F63" t="s">
-        <v>80</v>
       </c>
       <c r="G63" t="s">
         <v>9</v>
@@ -2094,19 +2106,19 @@
         <v>91</v>
       </c>
       <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C64" s="1">
-        <v>44063</v>
-      </c>
       <c r="D64" s="1">
+        <v>44063</v>
+      </c>
+      <c r="E64" s="1">
         <v>44062</v>
       </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
-        <v>80</v>
+      <c r="F64">
+        <v>0</v>
       </c>
       <c r="G64" t="s">
         <v>9</v>
@@ -2117,19 +2129,19 @@
         <v>92</v>
       </c>
       <c r="B65" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C65" s="1">
+      <c r="D65" s="1">
         <v>44047</v>
       </c>
-      <c r="D65" s="1">
-        <v>44063</v>
-      </c>
-      <c r="E65">
+      <c r="E65" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F65">
         <v>160</v>
-      </c>
-      <c r="F65" t="s">
-        <v>80</v>
       </c>
       <c r="G65" t="s">
         <v>9</v>
@@ -2142,17 +2154,17 @@
       <c r="B66" t="s">
         <v>83</v>
       </c>
-      <c r="C66" s="1">
-        <v>44063</v>
+      <c r="C66" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D66" s="1">
         <v>44063</v>
       </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66" t="s">
-        <v>84</v>
+      <c r="E66" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
       </c>
       <c r="G66" t="s">
         <v>9</v>
@@ -2163,19 +2175,19 @@
         <v>96</v>
       </c>
       <c r="B67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C67" s="1">
+      <c r="D67" s="1">
         <v>44047</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>44064</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>170</v>
-      </c>
-      <c r="F67" t="s">
-        <v>84</v>
       </c>
       <c r="G67" t="s">
         <v>9</v>
@@ -2186,19 +2198,19 @@
         <v>97</v>
       </c>
       <c r="B68" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="1">
+      <c r="D68" s="1">
         <v>44053</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>44060</v>
       </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68" t="s">
-        <v>84</v>
+      <c r="F68">
+        <v>0</v>
       </c>
       <c r="G68" t="s">
         <v>9</v>
@@ -2211,17 +2223,17 @@
       <c r="B69" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="1">
         <v>44043</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>44052</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>90</v>
-      </c>
-      <c r="F69" t="s">
-        <v>88</v>
       </c>
       <c r="G69" t="s">
         <v>9</v>
@@ -2232,19 +2244,19 @@
         <v>99</v>
       </c>
       <c r="B70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C70" s="1">
-        <v>44063</v>
-      </c>
       <c r="D70" s="1">
         <v>44063</v>
       </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
-        <v>88</v>
+      <c r="E70" s="1">
+        <v>44063</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
       </c>
       <c r="G70" t="s">
         <v>9</v>
@@ -2254,20 +2266,20 @@
       <c r="A71">
         <v>100</v>
       </c>
-      <c r="B71">
+      <c r="B71" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="3">
         <v>1984</v>
       </c>
-      <c r="C71" s="1">
+      <c r="D71" s="1">
         <v>44047</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>44064</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>170</v>
-      </c>
-      <c r="F71" t="s">
-        <v>90</v>
       </c>
       <c r="G71" t="s">
         <v>9</v>

</xml_diff>